<commit_message>
primeiro commit, falta ajustes
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,634 +464,405 @@
           <t>Resposta</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>TipoPergunta</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Qual é a capital da França?</t>
+          <t>Qual filme ganhou o Oscar de Melhor Filme em 2020?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Parasita</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Londres</t>
+          <t>1917</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Berlim</t>
+          <t>Coringa</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Roma</t>
+          <t>Era Uma Vez em Hollywood</t>
         </is>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Qual é o resultado de 8 + 5?</t>
+          <t>Quem é o protagonista da série 'Breaking Bad'?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Walter White</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>Jesse Pinkman</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>Saul Goodman</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>Hank Schrader</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Quem pintou a Mona Lisa?</t>
+          <t>Qual é o último livro da série 'Harry Potter'?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Picasso</t>
+          <t>As Relíquias da Morte</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Da Vinci</t>
+          <t>O Prisioneiro de Azkaban</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Van Gogh</t>
+          <t>A Ordem da Fênix</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Warhol</t>
+          <t>O Enigma do Príncipe</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Quanto é 6 multiplicado por 7?</t>
+          <t>Quem pintou a Mona Lisa?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>Leonardo da Vinci</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>Vincent van Gogh</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>Pablo Picasso</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>Claude Monet</t>
         </is>
       </c>
       <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Qual é o maior planeta do sistema solar?</t>
+          <t>Qual é a técnica artística de Pablo Picasso?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Marte</t>
+          <t>Cubismo</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Saturno</t>
+          <t>Impressionismo</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Júpiter</t>
+          <t>Realismo</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Vênus</t>
+          <t>Surrealismo</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Quem escreveu a obra 'Dom Quixote'?</t>
+          <t>Quem é o autor da obra 'Dom Quixote'?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Machado de Assis</t>
+          <t>Miguel de Cervantes</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Miguel de Cervantes</t>
+          <t>William Shakespeare</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Jorge Luis Borges</t>
+          <t>Charles Dickens</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Gabriel García Márquez</t>
+          <t>Jane Austen</t>
         </is>
       </c>
       <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Qual é a fórmula química da água?</t>
+          <t>O que é a teoria da relatividade de Einstein?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>H2O</t>
+          <t>Teoria da relatividade restrita</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Teoria da gravidade</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NaCl</t>
+          <t>Teoria da evolução</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CH4</t>
+          <t>Teoria da luz</t>
         </is>
       </c>
       <c r="F8" t="n">
         <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Quem foi o primeiro presidente dos Estados Unidos?</t>
+          <t>Quem foi o primeiro homem a pisar na lua?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>George Washington</t>
+          <t>Neil Armstrong</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Abraham Lincoln</t>
+          <t>Buzz Aldrin</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Thomas Jefferson</t>
+          <t>Yuri Gagarin</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>John F. Kennedy</t>
+          <t>John Glenn</t>
         </is>
       </c>
       <c r="F9" t="n">
         <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qual é o resultado de 4 ao cubo?</t>
+          <t>Qual é a fórmula química da água?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>H2O</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>O2</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>CH4</t>
         </is>
       </c>
       <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Qual é a capital da Rússia?</t>
+          <t>Qual país sediou a Copa do Mundo de 2018?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Moscou</t>
+          <t>Rússia</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>São Petersburgo</t>
+          <t>Alemanha</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Kiev</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Varsóvia</t>
+          <t>França</t>
         </is>
       </c>
       <c r="F11" t="n">
         <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Quem descobriu a teoria da relatividade?</t>
+          <t>Quem é considerado o melhor jogador de futebol de todos os tempos?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Isaac Newton</t>
+          <t>Pelé</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Galileu Galilei</t>
+          <t>Lionel Messi</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t>Cristiano Ronaldo</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Nikola Tesla</t>
+          <t>Diego Maradona</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Qual é o símbolo químico do ouro?</t>
+          <t>Em que esporte Michael Phelps se destacou nos Jogos Olímpicos?</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Au</t>
+          <t>Natação</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ag</t>
+          <t>Atletismo</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Cu</t>
+          <t>Ciclismo</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Fe</t>
+          <t>Ginástica</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Quem foi o autor da obra 'Romeu e Julieta'?</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>William Shakespeare</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Charles Dickens</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Mark Twain</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Jane Austen</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Qual é a capital do Brasil?</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Rio de Janeiro</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Brasília</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>São Paulo</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Qual é o resultado de 9 dividido por 3?</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Quem pintou a obra 'A Noite Estrelada'?</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Leonardo da Vinci</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Michelangelo</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Salvador Dalí</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Vincent van Gogh</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Qual é o maior oceano do mundo?</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Atlântico</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Índico</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Pacífico</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Ártico</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Qual é o resultado de 2 elevado a 8?</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>256</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Quem escreveu a obra '1984'?</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>George Orwell</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Aldous Huxley</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Ernest Hemingway</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>F. Scott Fitzgerald</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Qual é o resultado de 15 menos 7?</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Quem foi o pintor do quadro 'A Última Ceia'?</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Pablo Picasso</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Salvador Dalí</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Michelangelo</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Leonardo da Vinci</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
+      <c r="G13" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>